<commit_message>
delete nota value import
</commit_message>
<xml_diff>
--- a/public/import_template.xlsx
+++ b/public/import_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\nota-penjualan\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6A5D4F-2F6B-420A-9C8A-82106F7CA9B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1015F4-29E5-4E1F-99B3-A82DA5B507A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5D552E7F-2254-40BA-9E62-31582A1D301C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>golongan</t>
   </si>
@@ -51,31 +51,13 @@
     <t>THREE</t>
   </si>
   <si>
-    <t>no_nota</t>
-  </si>
-  <si>
-    <t>00001</t>
-  </si>
-  <si>
-    <t>00002</t>
-  </si>
-  <si>
     <t>ADEK012</t>
   </si>
   <si>
     <t>ADEK014</t>
   </si>
   <si>
-    <t>00003</t>
-  </si>
-  <si>
     <t>ADEK015</t>
-  </si>
-  <si>
-    <t>00004</t>
-  </si>
-  <si>
-    <t>00005</t>
   </si>
   <si>
     <t>ADEK017</t>
@@ -85,7 +67,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,8 +83,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,6 +100,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -128,13 +122,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,7 +449,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,9 +473,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -495,9 +490,7 @@
       <c r="D3" s="2">
         <v>17852</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -523,7 +516,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -536,9 +529,7 @@
       <c r="D7" s="2">
         <v>17852</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -564,7 +555,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -577,9 +568,7 @@
       <c r="D11" s="2">
         <v>17852</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -605,7 +594,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -618,9 +607,7 @@
       <c r="D15" s="2">
         <v>17852</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -646,7 +633,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -659,9 +646,7 @@
       <c r="D19" s="2">
         <v>17852</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">

</xml_diff>